<commit_message>
Se agrego la relacion entre cliente y eventos.
</commit_message>
<xml_diff>
--- a/ARCHIVOS/Terraza API.xlsx
+++ b/ARCHIVOS/Terraza API.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5271DD87-A142-4D77-BC55-D993710880D9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{358D3CB2-2CA8-4EF2-84D2-D8A1ED8CED06}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,12 +408,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
@@ -425,6 +419,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,13 +723,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -845,13 +845,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -952,13 +952,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -1059,13 +1059,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -1166,13 +1166,13 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -1256,79 +1256,79 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="7" t="s">
+      <c r="B40" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="7" t="s">
+      <c r="D40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9" t="s">
+      <c r="C41" s="7"/>
+      <c r="D41" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="9" t="s">
+      <c r="D42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="9" t="s">
+      <c r="D43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="12"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">

</xml_diff>